<commit_message>
novas frutas e sementes
</commit_message>
<xml_diff>
--- a/Imagens/Sementes Individuais/Dados organizados.xlsx
+++ b/Imagens/Sementes Individuais/Dados organizados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="150">
   <si>
     <t>castanha+ervilha</t>
   </si>
@@ -128,24 +128,15 @@
     <t>86.402496 - 99.943062</t>
   </si>
   <si>
-    <t>47 - 0</t>
-  </si>
-  <si>
     <t>138.879773 - 178.652124</t>
   </si>
   <si>
     <t>7149.000000 - 11273.000000</t>
   </si>
   <si>
-    <t>62 - 0</t>
-  </si>
-  <si>
     <t>4093.000000 - 4715.000000</t>
   </si>
   <si>
-    <t>24 - 0</t>
-  </si>
-  <si>
     <t>74.096514 - 87.412932</t>
   </si>
   <si>
@@ -155,63 +146,9 @@
     <t>27.327713 - 38.529839</t>
   </si>
   <si>
-    <t>87 - 0</t>
-  </si>
-  <si>
-    <t>140.000000 - 8543.000000</t>
-  </si>
-  <si>
-    <t>149 - 0</t>
-  </si>
-  <si>
-    <t>34 - 0</t>
-  </si>
-  <si>
     <t>0 - 0</t>
   </si>
   <si>
-    <t>30.853284 - 123.808552</t>
-  </si>
-  <si>
-    <t>84 - 68</t>
-  </si>
-  <si>
-    <t>52 - 36</t>
-  </si>
-  <si>
-    <t>48 - 32</t>
-  </si>
-  <si>
-    <t>134 - 87</t>
-  </si>
-  <si>
-    <t>112 - 65</t>
-  </si>
-  <si>
-    <t>112 - 50</t>
-  </si>
-  <si>
-    <t>101 - 39</t>
-  </si>
-  <si>
-    <t>132 - 108</t>
-  </si>
-  <si>
-    <t>47 - 23</t>
-  </si>
-  <si>
-    <t>146 - 59</t>
-  </si>
-  <si>
-    <t>119 - 32</t>
-  </si>
-  <si>
-    <t>overlap de area: cereja</t>
-  </si>
-  <si>
-    <t>overlap de area: amendoim</t>
-  </si>
-  <si>
     <t>dados juninho:</t>
   </si>
   <si>
@@ -248,9 +185,6 @@
     <t>164.046699 - 224.145401</t>
   </si>
   <si>
-    <t>129 - 68</t>
-  </si>
-  <si>
     <t>98 - 37</t>
   </si>
   <si>
@@ -312,6 +246,234 @@
   </si>
   <si>
     <t>103 - 51</t>
+  </si>
+  <si>
+    <t>5719.000000 - 8543.000000</t>
+  </si>
+  <si>
+    <t>101.731897 - 123.808552</t>
+  </si>
+  <si>
+    <t>64 - 84</t>
+  </si>
+  <si>
+    <t>33 - 52</t>
+  </si>
+  <si>
+    <t>33 - 48</t>
+  </si>
+  <si>
+    <t>0 - 192</t>
+  </si>
+  <si>
+    <t>123 - 134</t>
+  </si>
+  <si>
+    <t>91 - 112</t>
+  </si>
+  <si>
+    <t>26 - 47</t>
+  </si>
+  <si>
+    <t>90 - 112</t>
+  </si>
+  <si>
+    <t>71 - 101</t>
+  </si>
+  <si>
+    <t>31 - 62</t>
+  </si>
+  <si>
+    <t>117 - 132</t>
+  </si>
+  <si>
+    <t>4 '- 47</t>
+  </si>
+  <si>
+    <t>4 '- 24</t>
+  </si>
+  <si>
+    <t>111 - 146</t>
+  </si>
+  <si>
+    <t>96 - 119</t>
+  </si>
+  <si>
+    <t>63 - 87</t>
+  </si>
+  <si>
+    <t>128 - 149</t>
+  </si>
+  <si>
+    <t>14 - 34</t>
+  </si>
+  <si>
+    <t>azeitona+uva</t>
+  </si>
+  <si>
+    <t>azeitona+uvadedo</t>
+  </si>
+  <si>
+    <t>azeitona+tomate</t>
+  </si>
+  <si>
+    <t>azeitona+feijao</t>
+  </si>
+  <si>
+    <t>azeitona+uvapassa</t>
+  </si>
+  <si>
+    <t>uva+uvadedo</t>
+  </si>
+  <si>
+    <t>uva+tomate</t>
+  </si>
+  <si>
+    <t>uva+feijao</t>
+  </si>
+  <si>
+    <t>uva+uvapassa</t>
+  </si>
+  <si>
+    <t>uvadedo+tomate</t>
+  </si>
+  <si>
+    <t>uvadedo+feijao</t>
+  </si>
+  <si>
+    <t>uvadedo+uvapassa</t>
+  </si>
+  <si>
+    <t>tomate+feijao</t>
+  </si>
+  <si>
+    <t>tomate+uvapassa</t>
+  </si>
+  <si>
+    <t>feijao+uvapassa</t>
+  </si>
+  <si>
+    <t>uva</t>
+  </si>
+  <si>
+    <t>uvadedo</t>
+  </si>
+  <si>
+    <t>tomate</t>
+  </si>
+  <si>
+    <t>feijao</t>
+  </si>
+  <si>
+    <t>uvapassa</t>
+  </si>
+  <si>
+    <t>dados nova base</t>
+  </si>
+  <si>
+    <t>Azeitona</t>
+  </si>
+  <si>
+    <t>Tomate</t>
+  </si>
+  <si>
+    <t>Uva</t>
+  </si>
+  <si>
+    <t>UvaDedo</t>
+  </si>
+  <si>
+    <t>UvaPassa</t>
+  </si>
+  <si>
+    <t>30144.000000 - 38045.000000</t>
+  </si>
+  <si>
+    <t>223.858671 - 258.183849</t>
+  </si>
+  <si>
+    <t>148 - 191</t>
+  </si>
+  <si>
+    <t>113 - 141</t>
+  </si>
+  <si>
+    <t>65 - 80</t>
+  </si>
+  <si>
+    <t>4326.000000 - 6109.000000</t>
+  </si>
+  <si>
+    <t>84 - 93</t>
+  </si>
+  <si>
+    <t>88 - 99</t>
+  </si>
+  <si>
+    <t>91 - 100</t>
+  </si>
+  <si>
+    <t>93.454240 - 113.789051</t>
+  </si>
+  <si>
+    <t>59896.000000 - 72297.000000</t>
+  </si>
+  <si>
+    <t>229 - 255</t>
+  </si>
+  <si>
+    <t>91 - 103</t>
+  </si>
+  <si>
+    <t>56 - 66</t>
+  </si>
+  <si>
+    <t>290.418635 - 319.505983</t>
+  </si>
+  <si>
+    <t>29510.000000 - 49093.000000</t>
+  </si>
+  <si>
+    <t>171 - 189</t>
+  </si>
+  <si>
+    <t>89 - 95</t>
+  </si>
+  <si>
+    <t>94 - 100</t>
+  </si>
+  <si>
+    <t>197.470177 - 275.799963</t>
+  </si>
+  <si>
+    <t>32126.000000 - 43938.000000</t>
+  </si>
+  <si>
+    <t>88 - 97</t>
+  </si>
+  <si>
+    <t>93 - 100</t>
+  </si>
+  <si>
+    <t>97 - 104</t>
+  </si>
+  <si>
+    <t>307.870192 - 394.662647</t>
+  </si>
+  <si>
+    <t>95.945505 - 153.079598</t>
+  </si>
+  <si>
+    <t>206 - 224</t>
+  </si>
+  <si>
+    <t>140 - 155</t>
+  </si>
+  <si>
+    <t>51 - 65</t>
+  </si>
+  <si>
+    <t>5666.000000 - 11201.000000</t>
   </si>
 </sst>
 </file>
@@ -327,7 +489,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +556,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -422,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -465,6 +633,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -751,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:T33"/>
+  <dimension ref="B4:T44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E36" sqref="E36"/>
+    <sheetView tabSelected="1" topLeftCell="D29" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,7 +1320,7 @@
       <c r="T13" s="7"/>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D14" s="1"/>
@@ -1178,23 +1358,23 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="E15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>37</v>
+      <c r="F15" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>85</v>
       </c>
       <c r="N15" s="10" t="s">
         <v>18</v>
@@ -1219,26 +1399,23 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C16" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>34</v>
+      <c r="D16" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="F16" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="I16" s="15" t="s">
+        <v>40</v>
       </c>
       <c r="N16" s="10" t="s">
         <v>19</v>
@@ -1259,26 +1436,23 @@
       <c r="T16" s="7"/>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C17" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>43</v>
+      <c r="D17" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I17" s="15" t="s">
+        <v>82</v>
       </c>
       <c r="N17" s="11" t="s">
         <v>20</v>
@@ -1301,23 +1475,23 @@
       </c>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D18" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>51</v>
+      <c r="D18" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="I18" s="17" t="s">
+        <v>88</v>
       </c>
       <c r="N18" s="11" t="s">
         <v>21</v>
@@ -1338,23 +1512,23 @@
       </c>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="D19" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>39</v>
+      <c r="D19" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E19" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="G19" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="H19" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I19" s="15" t="s">
+        <v>78</v>
       </c>
       <c r="N19" s="1" t="s">
         <v>6</v>
@@ -1380,27 +1554,80 @@
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>48</v>
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>47</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+      <c r="O24" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="P24" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="R24" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="S24" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N25" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="O25" s="3"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="R25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="T25" s="7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N26" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="O26" s="3"/>
+      <c r="P26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="5"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="7"/>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C27" s="2" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1" t="s">
@@ -1418,128 +1645,409 @@
       <c r="I27" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="N27" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="O27" s="3"/>
+      <c r="P27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="5"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="7"/>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="F28" s="14" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>76</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="O28" s="3"/>
+      <c r="P28" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="5"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="7"/>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D29" s="1" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>76</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="O29" s="3"/>
+      <c r="P29" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="7"/>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D30" s="1" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>72</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="N30" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="O30" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="7"/>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D31" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="G31" s="13" t="s">
-        <v>89</v>
-      </c>
       <c r="H31" s="13" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>90</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="N31" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="O31" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="7"/>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D32" s="1" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="I32" s="13" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="N32" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="O32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="7"/>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
       <c r="D33" s="1" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="I33" s="13" t="s">
-        <v>86</v>
+        <v>64</v>
+      </c>
+      <c r="N33" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="O33" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="7"/>
+    </row>
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N34" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="O34" s="3"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="7"/>
+    </row>
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N35" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="O35" s="3"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="7"/>
+    </row>
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N36" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="O36" s="3"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="7"/>
+    </row>
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="N37" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="O37" s="3"/>
+      <c r="P37" s="5"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="7"/>
+    </row>
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N38" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="O38" s="3"/>
+      <c r="P38" s="5"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="5"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="7"/>
+    </row>
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D39" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H39" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="O39" s="3"/>
+      <c r="P39" s="5"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="5"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="7"/>
+    </row>
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="H40" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="I40" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D42" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E42" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42" s="13" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="43" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D43" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="44" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="D44" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="H44" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="I44" s="13" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>